<commit_message>
Add time sheet Golf
</commit_message>
<xml_diff>
--- a/Timesheet and MOM/Timesheet_reives 24092015.xlsx
+++ b/Timesheet and MOM/Timesheet_reives 24092015.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="810" windowWidth="19575" windowHeight="7080" activeTab="5"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="136">
   <si>
     <t>วิธีการกรอก</t>
   </si>
@@ -384,10 +384,6 @@
 - ทวนสอบโครงร่างหัวข้อ Proposal จากเอกสารคำแนะนำในการจัดทำเอกสาร </t>
   </si>
   <si>
-    <t xml:space="preserve">- ประชุมปรึกษาปัญหาที่เกิดจากการทำงานรอบที่แล้ว มอบหมายงาน และอธิบายเนื้องานที่ได้รับมอบหมายกันอาทิตย์นี้
--  </t>
-  </si>
-  <si>
     <t>ข้อมูลเนื้อหาที่จะทำงานมีข้อมูลไม่ครบด้วยทำให้การประชุมยังไม่มีประสิธิภาพมากพอ ดังนั้นก่อนการปะชุมในวันอาทิตย์ของทุกสัปกดาห์ ทุกคนในทีมจะต้องรวบรวมคำแนะนำจากการส่งงานรอบที่แล้ว และเรื่องที่จะทำงานส่งในรอบต่อไป เพื่อในการประชุมครั้งต่อไปทีมงานจะได้มีข้อมูลมาปรึกษาและช่วยกันหาคำตอบได้</t>
   </si>
   <si>
@@ -474,6 +470,16 @@
   </si>
   <si>
     <t>อ่านและศึกษาเพิ่มเติมจากเอกสารคำแนะในการจัดทำเอกสาร</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- ประชุมปรึกษาปัญหาที่เกิดจากการทำงานรอบที่แล้ว มอบหมายงาน และอธิบายเนื้องานที่ได้รับมอบหมายกันอาทิตย์นี้
+-  ทวนสอบ Proposal </t>
+  </si>
+  <si>
+    <t>ทวนเอกสารและข้อความที่ขาดเหลือ โดยมีการแบ่งงานในการประชุมกัน</t>
+  </si>
+  <si>
+    <t>เวลาในการทำงานของแต่ล่ะคนไม่ตรงกัน จึงทำให้การประชุมในบางครั้งอาจจะไม่ครบ</t>
   </si>
 </sst>
 </file>
@@ -1716,7 +1722,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H15" s="25" t="s">
         <v>72</v>
@@ -2156,7 +2162,7 @@
   </sheetPr>
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A10" zoomScale="80" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -2232,7 +2238,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
@@ -2311,7 +2317,7 @@
         <v>36</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D10" s="23">
         <v>3</v>
@@ -2324,10 +2330,10 @@
         <v>5</v>
       </c>
       <c r="G10" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="H10" s="25" t="s">
         <v>114</v>
-      </c>
-      <c r="H10" s="25" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="152.25" x14ac:dyDescent="0.2">
@@ -2338,7 +2344,7 @@
         <v>52</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D11" s="23">
         <v>4</v>
@@ -2351,10 +2357,10 @@
         <v>6</v>
       </c>
       <c r="G11" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="H11" s="25" t="s">
         <v>117</v>
-      </c>
-      <c r="H11" s="25" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="87" x14ac:dyDescent="0.2">
@@ -2365,7 +2371,7 @@
         <v>45</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D12" s="23">
         <v>3</v>
@@ -2378,10 +2384,10 @@
         <v>5</v>
       </c>
       <c r="G12" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="H12" s="25" t="s">
         <v>120</v>
-      </c>
-      <c r="H12" s="25" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2392,7 +2398,7 @@
         <v>57</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D13" s="23">
         <v>3</v>
@@ -2405,10 +2411,10 @@
         <v>5</v>
       </c>
       <c r="G13" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="H13" s="25" t="s">
         <v>123</v>
-      </c>
-      <c r="H13" s="25" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2419,7 +2425,7 @@
         <v>84</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D14" s="23">
         <v>4</v>
@@ -2432,10 +2438,10 @@
         <v>6</v>
       </c>
       <c r="G14" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="H14" s="25" t="s">
         <v>126</v>
-      </c>
-      <c r="H14" s="25" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="21.75" x14ac:dyDescent="0.5">
@@ -2475,7 +2481,7 @@
     <mergeCell ref="G8:G9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="68" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="69" orientation="landscape" r:id="rId1"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="8" max="1048575" man="1"/>
   </colBreaks>
@@ -2501,7 +2507,7 @@
   </sheetPr>
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -2851,8 +2857,8 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -2902,7 +2908,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="21.75" x14ac:dyDescent="0.5">
@@ -3001,7 +3007,7 @@
         <v>45</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D12" s="23">
         <v>3</v>
@@ -3014,10 +3020,10 @@
         <v>10</v>
       </c>
       <c r="G12" s="31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="134.25" customHeight="1" x14ac:dyDescent="0.5">
@@ -3028,18 +3034,24 @@
         <v>57</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="D13" s="23"/>
+        <v>133</v>
+      </c>
+      <c r="D13" s="23">
+        <v>3</v>
+      </c>
       <c r="E13" s="23">
         <v>2</v>
       </c>
       <c r="F13" s="23">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G13" s="31"/>
-      <c r="H13" s="25"/>
+        <v>5</v>
+      </c>
+      <c r="G13" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="H13" s="25" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="165.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A14" s="33">
@@ -3049,7 +3061,7 @@
         <v>84</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D14" s="23">
         <v>4</v>
@@ -3062,10 +3074,10 @@
         <v>6</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H14" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="21.75" x14ac:dyDescent="0.5">
@@ -3078,7 +3090,7 @@
       <c r="E15" s="38"/>
       <c r="F15" s="23">
         <f>SUM(F10:F14)</f>
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G15" s="24"/>
       <c r="H15" s="24"/>

</xml_diff>